<commit_message>
Adds the features of the java code "data capes"
There are still some fixes to do and comments to write
</commit_message>
<xml_diff>
--- a/resources/synonyms/journals_synonyms.xlsx
+++ b/resources/synonyms/journals_synonyms.xlsx
@@ -708,10 +708,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-&quot;R$&quot;* #,##0_-;\-&quot;R$&quot;* #,##0_-;_-&quot;R$&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-&quot;R$&quot;* #,##0.00_-;\-&quot;R$&quot;* #,##0.00_-;_-&quot;R$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="178" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="_-&quot;R$&quot;* #,##0.00_-;\-&quot;R$&quot;* #,##0.00_-;_-&quot;R$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-&quot;R$&quot;* #,##0_-;\-&quot;R$&quot;* #,##0_-;_-&quot;R$&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -723,59 +723,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -784,6 +732,13 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -798,7 +753,7 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -813,7 +768,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -821,7 +776,60 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -844,14 +852,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -859,10 +859,10 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -875,31 +875,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -911,138 +1049,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1050,12 +1056,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1084,6 +1084,30 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -1096,8 +1120,23 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1117,45 +1156,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -1174,150 +1174,153 @@
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="27" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1642,966 +1645,1080 @@
   <dimension ref="A1:C118"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="A1" sqref="A1:C118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.2857142857143" defaultRowHeight="12.75" outlineLevelCol="2"/>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
+      <c r="C1" s="1"/>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
+      <c r="C3" s="1"/>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
+      <c r="C4" s="1"/>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
+      <c r="C5" s="1"/>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
+      <c r="C6" s="1"/>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
+      <c r="C7" s="1"/>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s">
+      <c r="C8" s="1"/>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="s">
+      <c r="C9" s="1"/>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" t="s">
+      <c r="C10" s="1"/>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" t="s">
+      <c r="C11" s="1"/>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" t="s">
+      <c r="C12" s="1"/>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" t="s">
+      <c r="C13" s="1"/>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" t="s">
+      <c r="C14" s="1"/>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" t="s">
+      <c r="C15" s="1"/>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" t="s">
+      <c r="C16" s="1"/>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" t="s">
+      <c r="C17" s="1"/>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" t="s">
+      <c r="C18" s="1"/>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" t="s">
+      <c r="C19" s="1"/>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" t="s">
+      <c r="C20" s="1"/>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" t="s">
+      <c r="C21" s="1"/>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" t="s">
+      <c r="C22" s="1"/>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" t="s">
+      <c r="C23" s="1"/>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25" t="s">
+      <c r="C24" s="1"/>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="26" spans="1:2">
-      <c r="A26" t="s">
+      <c r="C25" s="1"/>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="27" spans="1:2">
-      <c r="A27" t="s">
+      <c r="C26" s="1"/>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="1" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="28" spans="1:2">
-      <c r="A28" t="s">
+      <c r="C27" s="1"/>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="29" spans="1:2">
-      <c r="A29" t="s">
+      <c r="C28" s="1"/>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="30" spans="1:2">
-      <c r="A30" t="s">
+      <c r="C29" s="1"/>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="1" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="31" spans="1:2">
-      <c r="A31" t="s">
+      <c r="C30" s="1"/>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="1" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="32" spans="1:2">
-      <c r="A32" t="s">
+      <c r="C31" s="1"/>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="33" spans="1:2">
-      <c r="A33" t="s">
+      <c r="C32" s="1"/>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="1" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="34" spans="1:2">
-      <c r="A34" t="s">
+      <c r="C33" s="1"/>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="1" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="35" spans="1:2">
-      <c r="A35" t="s">
+      <c r="C34" s="1"/>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="1" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="36" spans="1:2">
-      <c r="A36" t="s">
+      <c r="C35" s="1"/>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="1" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="37" spans="1:2">
-      <c r="A37" t="s">
+      <c r="C36" s="1"/>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="1" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="38" spans="1:2">
-      <c r="A38" t="s">
+      <c r="C37" s="1"/>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="1" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="39" spans="1:2">
-      <c r="A39" t="s">
+      <c r="C38" s="1"/>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="1" t="s">
         <v>75</v>
       </c>
+      <c r="C39" s="1"/>
     </row>
     <row r="40" spans="1:3">
-      <c r="A40" t="s">
+      <c r="A40" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C40" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
-      <c r="A41" t="s">
+    <row r="41" spans="1:3">
+      <c r="A41" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="1" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="42" spans="1:2">
-      <c r="A42" t="s">
+      <c r="C41" s="1"/>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="1" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="43" spans="1:2">
-      <c r="A43" t="s">
+      <c r="C42" s="1"/>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="1" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="44" spans="1:2">
-      <c r="A44" t="s">
+      <c r="C43" s="1"/>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" s="1" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="45" spans="1:2">
-      <c r="A45" t="s">
+      <c r="C44" s="1"/>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B45" s="1" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="46" spans="1:2">
-      <c r="A46" t="s">
+      <c r="C45" s="1"/>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B46" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="47" spans="1:2">
-      <c r="A47" t="s">
+      <c r="C46" s="1"/>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B47" s="1" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="48" spans="1:2">
-      <c r="A48" t="s">
+      <c r="C47" s="1"/>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B48" s="1" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="49" spans="1:2">
-      <c r="A49" t="s">
+      <c r="C48" s="1"/>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B49" s="1" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="50" spans="1:2">
-      <c r="A50" t="s">
+      <c r="C49" s="1"/>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B50" s="1" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="51" spans="1:2">
-      <c r="A51" t="s">
+      <c r="C50" s="1"/>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B51" s="1" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="52" spans="1:2">
-      <c r="A52" t="s">
+      <c r="C51" s="1"/>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B52" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="53" spans="1:2">
-      <c r="A53" t="s">
+      <c r="C52" s="1"/>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B53" s="1" t="s">
         <v>102</v>
       </c>
+      <c r="C53" s="1"/>
     </row>
     <row r="54" spans="1:3">
-      <c r="A54" t="s">
+      <c r="A54" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B54" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C54" s="1" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="55" spans="1:2">
-      <c r="A55" t="s">
+    <row r="55" spans="1:3">
+      <c r="A55" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B55" s="1" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="56" spans="1:2">
-      <c r="A56" t="s">
+      <c r="C55" s="1"/>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B56" s="1" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="57" spans="1:2">
-      <c r="A57" t="s">
+      <c r="C56" s="1"/>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B57" s="1" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="58" spans="1:2">
-      <c r="A58" t="s">
+      <c r="C57" s="1"/>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B58" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="59" spans="1:2">
-      <c r="A59" t="s">
+      <c r="C58" s="1"/>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B59" s="1" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="60" spans="1:2">
-      <c r="A60" t="s">
+      <c r="C59" s="1"/>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B60" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="61" spans="1:2">
-      <c r="A61" t="s">
+      <c r="C60" s="1"/>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B61" s="1" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="62" spans="1:2">
-      <c r="A62" t="s">
+      <c r="C61" s="1"/>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="A62" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B62" s="1" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="63" spans="1:2">
-      <c r="A63" t="s">
+      <c r="C62" s="1"/>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B63" s="1" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="64" spans="1:2">
-      <c r="A64" t="s">
+      <c r="C63" s="1"/>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B64" s="1" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="65" spans="1:2">
-      <c r="A65" t="s">
+      <c r="C64" s="1"/>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B65" s="1" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="66" spans="1:2">
-      <c r="A66" t="s">
+      <c r="C65" s="1"/>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B66" s="1" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="67" spans="1:2">
-      <c r="A67" t="s">
+      <c r="C66" s="1"/>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B67" s="1" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="68" spans="1:2">
-      <c r="A68" t="s">
+      <c r="C67" s="1"/>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B68" s="1" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="69" spans="1:2">
-      <c r="A69" t="s">
+      <c r="C68" s="1"/>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B69" s="1" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="70" spans="1:2">
-      <c r="A70" t="s">
+      <c r="C69" s="1"/>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B70" s="1" t="s">
         <v>136</v>
       </c>
+      <c r="C70" s="1"/>
     </row>
     <row r="71" spans="1:3">
-      <c r="A71" t="s">
+      <c r="A71" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B71" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="C71" t="s">
+      <c r="C71" s="1" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="72" spans="1:2">
-      <c r="A72" t="s">
+    <row r="72" spans="1:3">
+      <c r="A72" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B72" s="1" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="73" spans="1:2">
-      <c r="A73" t="s">
+      <c r="C72" s="1"/>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="A73" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="B73" t="s">
+      <c r="B73" s="1" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="74" spans="1:2">
-      <c r="A74" t="s">
+      <c r="C73" s="1"/>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="A74" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B74" s="1" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="75" spans="1:2">
-      <c r="A75" t="s">
+      <c r="C74" s="1"/>
+    </row>
+    <row r="75" spans="1:3">
+      <c r="A75" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="B75" t="s">
+      <c r="B75" s="1" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="76" spans="1:2">
-      <c r="A76" t="s">
+      <c r="C75" s="1"/>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="A76" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="B76" t="s">
+      <c r="B76" s="1" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="77" spans="1:2">
-      <c r="A77" t="s">
+      <c r="C76" s="1"/>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="A77" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="B77" t="s">
+      <c r="B77" s="1" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="78" spans="1:2">
-      <c r="A78" t="s">
+      <c r="C77" s="1"/>
+    </row>
+    <row r="78" spans="1:3">
+      <c r="A78" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="B78" t="s">
+      <c r="B78" s="1" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="79" spans="1:2">
-      <c r="A79" t="s">
+      <c r="C78" s="1"/>
+    </row>
+    <row r="79" spans="1:3">
+      <c r="A79" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="B79" t="s">
+      <c r="B79" s="1" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="80" spans="1:2">
-      <c r="A80" t="s">
+      <c r="C79" s="1"/>
+    </row>
+    <row r="80" spans="1:3">
+      <c r="A80" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B80" s="1" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="81" spans="1:2">
-      <c r="A81" t="s">
+      <c r="C80" s="1"/>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="A81" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="B81" t="s">
+      <c r="B81" s="1" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="82" spans="1:2">
-      <c r="A82" t="s">
+      <c r="C81" s="1"/>
+    </row>
+    <row r="82" spans="1:3">
+      <c r="A82" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="B82" t="s">
+      <c r="B82" s="1" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="83" spans="1:2">
-      <c r="A83" t="s">
+      <c r="C82" s="1"/>
+    </row>
+    <row r="83" spans="1:3">
+      <c r="A83" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="B83" t="s">
+      <c r="B83" s="1" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="84" spans="1:2">
-      <c r="A84" t="s">
+      <c r="C83" s="1"/>
+    </row>
+    <row r="84" spans="1:3">
+      <c r="A84" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="B84" t="s">
+      <c r="B84" s="1" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="85" spans="1:2">
-      <c r="A85" t="s">
+      <c r="C84" s="1"/>
+    </row>
+    <row r="85" spans="1:3">
+      <c r="A85" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="B85" t="s">
+      <c r="B85" s="1" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="86" spans="1:2">
-      <c r="A86" t="s">
+      <c r="C85" s="1"/>
+    </row>
+    <row r="86" spans="1:3">
+      <c r="A86" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="B86" t="s">
+      <c r="B86" s="1" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="87" spans="1:2">
-      <c r="A87" t="s">
+      <c r="C86" s="1"/>
+    </row>
+    <row r="87" spans="1:3">
+      <c r="A87" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="B87" t="s">
+      <c r="B87" s="1" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="88" spans="1:2">
-      <c r="A88" t="s">
+      <c r="C87" s="1"/>
+    </row>
+    <row r="88" spans="1:3">
+      <c r="A88" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B88" t="s">
+      <c r="B88" s="1" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="89" spans="1:2">
-      <c r="A89" t="s">
+      <c r="C88" s="1"/>
+    </row>
+    <row r="89" spans="1:3">
+      <c r="A89" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B89" t="s">
+      <c r="B89" s="1" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="90" spans="1:2">
-      <c r="A90" t="s">
+      <c r="C89" s="1"/>
+    </row>
+    <row r="90" spans="1:3">
+      <c r="A90" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="B90" t="s">
+      <c r="B90" s="1" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="91" spans="1:2">
-      <c r="A91" t="s">
+      <c r="C90" s="1"/>
+    </row>
+    <row r="91" spans="1:3">
+      <c r="A91" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="B91" t="s">
+      <c r="B91" s="1" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="92" spans="1:2">
-      <c r="A92" t="s">
+      <c r="C91" s="1"/>
+    </row>
+    <row r="92" spans="1:3">
+      <c r="A92" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="B92" t="s">
+      <c r="B92" s="1" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="93" spans="1:2">
-      <c r="A93" t="s">
+      <c r="C92" s="1"/>
+    </row>
+    <row r="93" spans="1:3">
+      <c r="A93" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="B93" t="s">
+      <c r="B93" s="1" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="94" spans="1:2">
-      <c r="A94" t="s">
+      <c r="C93" s="1"/>
+    </row>
+    <row r="94" spans="1:3">
+      <c r="A94" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="B94" t="s">
+      <c r="B94" s="1" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="95" spans="1:2">
-      <c r="A95" t="s">
+      <c r="C94" s="1"/>
+    </row>
+    <row r="95" spans="1:3">
+      <c r="A95" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="B95" t="s">
+      <c r="B95" s="1" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="96" spans="1:2">
-      <c r="A96" t="s">
+      <c r="C95" s="1"/>
+    </row>
+    <row r="96" spans="1:3">
+      <c r="A96" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="B96" t="s">
+      <c r="B96" s="1" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="97" spans="1:2">
-      <c r="A97" t="s">
+      <c r="C96" s="1"/>
+    </row>
+    <row r="97" spans="1:3">
+      <c r="A97" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="B97" t="s">
+      <c r="B97" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="98" spans="1:2">
-      <c r="A98" t="s">
+      <c r="C97" s="1"/>
+    </row>
+    <row r="98" spans="1:3">
+      <c r="A98" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="B98" t="s">
+      <c r="B98" s="1" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="99" spans="1:2">
-      <c r="A99" t="s">
+      <c r="C98" s="1"/>
+    </row>
+    <row r="99" spans="1:3">
+      <c r="A99" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="B99" t="s">
+      <c r="B99" s="1" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="100" spans="1:2">
-      <c r="A100" t="s">
+      <c r="C99" s="1"/>
+    </row>
+    <row r="100" spans="1:3">
+      <c r="A100" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B100" t="s">
+      <c r="B100" s="1" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="101" spans="1:2">
-      <c r="A101" t="s">
+      <c r="C100" s="1"/>
+    </row>
+    <row r="101" spans="1:3">
+      <c r="A101" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="B101" t="s">
+      <c r="B101" s="1" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="102" spans="1:2">
-      <c r="A102" t="s">
+      <c r="C101" s="1"/>
+    </row>
+    <row r="102" spans="1:3">
+      <c r="A102" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="B102" t="s">
+      <c r="B102" s="1" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="103" spans="1:2">
-      <c r="A103" t="s">
+      <c r="C102" s="1"/>
+    </row>
+    <row r="103" spans="1:3">
+      <c r="A103" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="B103" t="s">
+      <c r="B103" s="1" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="104" spans="1:2">
-      <c r="A104" t="s">
+      <c r="C103" s="1"/>
+    </row>
+    <row r="104" spans="1:3">
+      <c r="A104" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="B104" t="s">
+      <c r="B104" s="1" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="105" spans="1:2">
-      <c r="A105" t="s">
+      <c r="C104" s="1"/>
+    </row>
+    <row r="105" spans="1:3">
+      <c r="A105" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="B105" t="s">
+      <c r="B105" s="1" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="106" spans="1:2">
-      <c r="A106" t="s">
+      <c r="C105" s="1"/>
+    </row>
+    <row r="106" spans="1:3">
+      <c r="A106" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B106" t="s">
+      <c r="B106" s="1" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="107" spans="1:2">
-      <c r="A107" t="s">
+      <c r="C106" s="1"/>
+    </row>
+    <row r="107" spans="1:3">
+      <c r="A107" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="B107" t="s">
+      <c r="B107" s="1" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="108" spans="1:2">
-      <c r="A108" t="s">
+      <c r="C107" s="1"/>
+    </row>
+    <row r="108" spans="1:3">
+      <c r="A108" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="B108" t="s">
+      <c r="B108" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="109" spans="1:2">
-      <c r="A109" t="s">
+      <c r="C108" s="1"/>
+    </row>
+    <row r="109" spans="1:3">
+      <c r="A109" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="B109" t="s">
+      <c r="B109" s="1" t="s">
         <v>210</v>
       </c>
+      <c r="C109" s="1"/>
     </row>
     <row r="110" spans="1:3">
-      <c r="A110" t="s">
+      <c r="A110" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="B110" t="s">
+      <c r="B110" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="C110" t="s">
+      <c r="C110" s="1" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="111" spans="1:2">
-      <c r="A111" t="s">
+    <row r="111" spans="1:3">
+      <c r="A111" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B111" t="s">
+      <c r="B111" s="1" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="112" spans="1:2">
-      <c r="A112" t="s">
+      <c r="C111" s="1"/>
+    </row>
+    <row r="112" spans="1:3">
+      <c r="A112" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="B112" t="s">
+      <c r="B112" s="1" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="113" spans="1:2">
-      <c r="A113" t="s">
+      <c r="C112" s="1"/>
+    </row>
+    <row r="113" spans="1:3">
+      <c r="A113" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="B113" t="s">
+      <c r="B113" s="1" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="114" spans="1:2">
-      <c r="A114" t="s">
+      <c r="C113" s="1"/>
+    </row>
+    <row r="114" spans="1:3">
+      <c r="A114" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="B114" t="s">
+      <c r="B114" s="1" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="115" spans="1:2">
-      <c r="A115" t="s">
+      <c r="C114" s="1"/>
+    </row>
+    <row r="115" spans="1:3">
+      <c r="A115" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="B115" t="s">
+      <c r="B115" s="1" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="116" spans="1:2">
-      <c r="A116" t="s">
+      <c r="C115" s="1"/>
+    </row>
+    <row r="116" spans="1:3">
+      <c r="A116" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="B116" t="s">
+      <c r="B116" s="1" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="117" spans="1:2">
-      <c r="A117" t="s">
+      <c r="C116" s="1"/>
+    </row>
+    <row r="117" spans="1:3">
+      <c r="A117" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="B117" t="s">
+      <c r="B117" s="1" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="118" spans="1:2">
-      <c r="A118" t="s">
+      <c r="C117" s="1"/>
+    </row>
+    <row r="118" spans="1:3">
+      <c r="A118" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="B118" t="s">
+      <c r="B118" s="1" t="s">
         <v>228</v>
       </c>
+      <c r="C118" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>